<commit_message>
Mise à jour du plan de tests
Mise à jour du plan de test et création d'une issue en conséquence.
</commit_message>
<xml_diff>
--- a/Unit_Test/plan_test.xlsx
+++ b/Unit_Test/plan_test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romain\Documents\GitHub\MT5\Unit_Test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20424"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de test" sheetId="1" r:id="rId1"/>
@@ -16,18 +21,18 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="174">
   <si>
     <t>Plan de tests</t>
   </si>
@@ -532,9 +537,6 @@
     <t>Adapter l'aspect du bouton en fnt de l'état de la piste</t>
   </si>
   <si>
-    <t>RAF</t>
-  </si>
-  <si>
     <t>Lecture d'une musique personnelle</t>
   </si>
   <si>
@@ -582,6 +584,9 @@
   </si>
   <si>
     <t>Une fenêtre s'affiche avec les informations du GitHub</t>
+  </si>
+  <si>
+    <t>KO</t>
   </si>
 </sst>
 </file>
@@ -651,11 +656,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -743,13 +748,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A6:H44" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A6:H44">
-    <filterColumn colId="6">
-      <filters blank="1">
-        <filter val="RAF"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A6:H44"/>
   <tableColumns count="8">
     <tableColumn id="1" name="N" dataDxfId="17"/>
     <tableColumn id="2" name="Module" dataDxfId="16"/>
@@ -1036,7 +1035,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1044,68 +1043,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.5" style="1"/>
+    <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1131,7 +1130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="26.25" hidden="1" customHeight="1">
+    <row r="7" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -1147,14 +1146,14 @@
       <c r="E7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>150</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28" hidden="1">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -1170,14 +1169,14 @@
       <c r="E8" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>146</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28" hidden="1">
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1193,14 +1192,14 @@
       <c r="E9" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>152</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28" hidden="1">
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -1223,7 +1222,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="28" hidden="1">
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28" hidden="1">
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1254,7 +1253,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>56</v>
@@ -1269,10 +1268,10 @@
         <v>151</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" hidden="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="28" hidden="1">
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1318,7 +1317,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="28" hidden="1">
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
@@ -1341,7 +1340,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="28" hidden="1">
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>63</v>
       </c>
@@ -1364,7 +1363,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="28">
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>74</v>
       </c>
@@ -1384,13 +1383,13 @@
         <v>153</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>75</v>
       </c>
@@ -1410,10 +1409,13 @@
         <v>154</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" hidden="1">
+        <v>173</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>78</v>
       </c>
@@ -1436,7 +1438,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1">
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>80</v>
       </c>
@@ -1459,7 +1461,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="42" hidden="1">
+    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>83</v>
       </c>
@@ -1482,7 +1484,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="42" hidden="1">
+    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>85</v>
       </c>
@@ -1505,7 +1507,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="28" hidden="1">
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
@@ -1519,7 +1521,7 @@
         <v>99</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>89</v>
@@ -1528,7 +1530,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="28" hidden="1">
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>90</v>
       </c>
@@ -1542,7 +1544,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>97</v>
@@ -1551,7 +1553,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="28" hidden="1">
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>91</v>
       </c>
@@ -1568,13 +1570,13 @@
         <v>108</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28" hidden="1">
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
@@ -1588,16 +1590,16 @@
         <v>51</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="G29" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="28" hidden="1">
+    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>93</v>
       </c>
@@ -1614,13 +1616,13 @@
         <v>109</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28" hidden="1">
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -1637,13 +1639,13 @@
         <v>109</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="28" hidden="1">
+    <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>95</v>
       </c>
@@ -1666,7 +1668,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>117</v>
       </c>
@@ -1686,13 +1688,13 @@
         <v>121</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" hidden="1">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>122</v>
       </c>
@@ -1715,7 +1717,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="28" hidden="1">
+    <row r="36" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>126</v>
       </c>
@@ -1738,7 +1740,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="28" hidden="1">
+    <row r="38" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>129</v>
       </c>
@@ -1749,7 +1751,7 @@
         <v>131</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>132</v>
@@ -1761,7 +1763,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>136</v>
       </c>
@@ -1778,10 +1780,13 @@
         <v>135</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="42" hidden="1">
+        <v>166</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>137</v>
       </c>
@@ -1789,10 +1794,10 @@
         <v>130</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>138</v>
@@ -1801,7 +1806,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>145</v>
       </c>
@@ -1814,22 +1819,25 @@
       <c r="E42" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="G42" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>142</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>151</v>
@@ -1860,19 +1868,19 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="28.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="70.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="61.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="70.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="61.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="45.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="1"/>
     <col min="8" max="8" width="14.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -1898,7 +1906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="78" customHeight="1">
+    <row r="2" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
@@ -1918,7 +1926,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="66.75" customHeight="1">
+    <row r="3" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -1938,7 +1946,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="84" customHeight="1">
+    <row r="4" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -1958,7 +1966,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
@@ -1978,7 +1986,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
@@ -1998,7 +2006,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="56">
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -2021,7 +2029,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -2062,12 +2070,12 @@
       <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2075,7 +2083,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2083,7 +2091,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2091,7 +2099,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2099,7 +2107,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2107,7 +2115,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2115,7 +2123,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2123,7 +2131,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2131,7 +2139,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2139,7 +2147,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2147,7 +2155,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>141</v>
       </c>

</xml_diff>